<commit_message>
add excel MMI chart
</commit_message>
<xml_diff>
--- a/other/wykresy.xlsx
+++ b/other/wykresy.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dawid\Documents\GitHub\EngineeringProject git\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD434D7F-C1BC-4524-846F-2F1A5745AB92}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0702269-B0D9-41D6-A027-EC2439ED840C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{09C2883A-FE89-41EB-9B4F-685F7054BFF8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{09C2883A-FE89-41EB-9B4F-685F7054BFF8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="ft4 i trab" sheetId="1" r:id="rId1"/>
+    <sheet name="mmi treatment" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>fT4 (pg/mL)</t>
   </si>
@@ -49,6 +50,27 @@
   </si>
   <si>
     <t>Pacjent nr 70</t>
+  </si>
+  <si>
+    <t>Pacjent nr 31</t>
+  </si>
+  <si>
+    <t>dni</t>
+  </si>
+  <si>
+    <t>dawka</t>
+  </si>
+  <si>
+    <t>suma</t>
+  </si>
+  <si>
+    <t>ilosc MMI</t>
+  </si>
+  <si>
+    <t>fT4 (pg/ml)</t>
+  </si>
+  <si>
+    <t>MMI (g/l)</t>
   </si>
 </sst>
 </file>
@@ -206,7 +228,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$5</c:f>
+              <c:f>'ft4 i trab'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -227,7 +249,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$B$4:$E$4</c:f>
+              <c:f>'ft4 i trab'!$B$4:$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -247,7 +269,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$B$5:$E$5</c:f>
+              <c:f>'ft4 i trab'!$B$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -277,7 +299,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$A$6</c:f>
+              <c:f>'ft4 i trab'!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -298,7 +320,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Arkusz1!$B$4:$E$4</c:f>
+              <c:f>'ft4 i trab'!$B$4:$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -318,7 +340,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$B$6:$E$6</c:f>
+              <c:f>'ft4 i trab'!$B$6:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -539,7 +561,678 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Zapotrzebowanie na lek pacjentów</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'mmi treatment'!$H$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MMI (g/l)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'mmi treatment'!$I$5:$L$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Pacjent nr 20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pacjent nr 31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pacjent nr 55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Pacjent nr 70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'mmi treatment'!$I$6:$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2B89-4BE3-8560-B038C3156CC2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="726611616"/>
+        <c:axId val="740307056"/>
+      </c:barChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'mmi treatment'!$H$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fT4 (pg/ml)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'mmi treatment'!$I$5:$L$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Pacjent nr 20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pacjent nr 31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pacjent nr 55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Pacjent nr 70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'mmi treatment'!$I$7:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>25.63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2B89-4BE3-8560-B038C3156CC2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="736885536"/>
+        <c:axId val="774973040"/>
+      </c:scatterChart>
+      <c:catAx>
+        <c:axId val="726611616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740307056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="740307056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400"/>
+                  <a:t>Ilość</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400" baseline="0"/>
+                  <a:t> MMI (g/l)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="726611616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="774973040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Ilość fT4 (pg/ml)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="736885536"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="736885536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="774973040"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1082,6 +1775,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1103,6 +2299,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A1ADB77-3BC4-459C-861F-A94D2B8827EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A380B849-366D-4BA8-AF45-D73928F79812}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1422,8 +2659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E740B4AC-0CE7-4C2F-ACA0-BEBF2EC352A3}">
   <dimension ref="A4:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,4 +2717,361 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66936F0A-2EF8-4566-8024-ADE8A81ED3E6}">
+  <dimension ref="A5:L27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>60</v>
+      </c>
+      <c r="C6">
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
+      <c r="E6">
+        <v>180</v>
+      </c>
+      <c r="F6">
+        <f>SUM(B6:E6)</f>
+        <v>360</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <f>F7/1000</f>
+        <v>4.8</v>
+      </c>
+      <c r="J6">
+        <f>F14/1000</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K6">
+        <f>F20/1000</f>
+        <v>4.8</v>
+      </c>
+      <c r="L6">
+        <f>F26/1000</f>
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f>SUM(B8:E8)</f>
+        <v>4800</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="5">
+        <v>25.63</v>
+      </c>
+      <c r="J7" s="5">
+        <v>26.43</v>
+      </c>
+      <c r="K7" s="5">
+        <v>27.01</v>
+      </c>
+      <c r="L7" s="5">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>B6*B7</f>
+        <v>1800</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:E8" si="0">C6*C7</f>
+        <v>1200</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>90</v>
+      </c>
+      <c r="C13">
+        <v>120</v>
+      </c>
+      <c r="D13">
+        <v>150</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f>SUM(B13:E13)</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <f>SUM(B15:E15)</f>
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <f>B13*B14</f>
+        <v>3600</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15" si="1">C13*C14</f>
+        <v>3600</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15" si="2">D13*D14</f>
+        <v>3000</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15" si="3">E13*E14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>60</v>
+      </c>
+      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="D19">
+        <v>60</v>
+      </c>
+      <c r="E19">
+        <v>180</v>
+      </c>
+      <c r="F19">
+        <f>SUM(B19:E19)</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <f>SUM(B21:E21)</f>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <f>B19*B20</f>
+        <v>1800</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21" si="4">C19*C20</f>
+        <v>1200</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21" si="5">D19*D20</f>
+        <v>900</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21" si="6">E19*E20</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>90</v>
+      </c>
+      <c r="D25">
+        <v>90</v>
+      </c>
+      <c r="E25">
+        <v>120</v>
+      </c>
+      <c r="F25">
+        <f>SUM(B25:E25)</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>15</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <f>SUM(B27:E27)</f>
+        <v>5550</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <f>B25*B26</f>
+        <v>1800</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27" si="7">C25*C26</f>
+        <v>1800</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ref="D27" si="8">D25*D26</f>
+        <v>1350</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ref="E27" si="9">E25*E26</f>
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
poprawki v3 bez rezultatów
</commit_message>
<xml_diff>
--- a/other/wykresy.xlsx
+++ b/other/wykresy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dawid\Documents\GitHub\EngineeringProject git\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0702269-B0D9-41D6-A027-EC2439ED840C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD7808B-72A4-4A91-8E28-2FEF779BA1DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{09C2883A-FE89-41EB-9B4F-685F7054BFF8}"/>
   </bookViews>
@@ -67,10 +67,10 @@
     <t>ilosc MMI</t>
   </si>
   <si>
-    <t>fT4 (pg/ml)</t>
+    <t>MMI (g/l)</t>
   </si>
   <si>
-    <t>MMI (g/l)</t>
+    <t>FT4 (pg/ml)</t>
   </si>
 </sst>
 </file>
@@ -732,7 +732,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>fT4 (pg/ml)</c:v>
+                  <c:v>FT4 (pg/ml)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1012,7 +1012,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Ilość fT4 (pg/ml)</a:t>
+                  <a:t>Ilość </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>F</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>T4 (pg/ml)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1107,6 +1115,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="774973040"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2723,8 +2732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66936F0A-2EF8-4566-8024-ADE8A81ED3E6}">
   <dimension ref="A5:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2781,7 +2790,7 @@
         <v>360</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I6">
         <f>F7/1000</f>
@@ -2821,7 +2830,7 @@
         <v>4800</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I7" s="5">
         <v>25.63</v>

</xml_diff>

<commit_message>
korekta 4.1 done - fix rezultaty (rozdział 6)
</commit_message>
<xml_diff>
--- a/other/wykresy.xlsx
+++ b/other/wykresy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dawid\Documents\GitHub\EngineeringProject git\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD7808B-72A4-4A91-8E28-2FEF779BA1DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD845985-AE6B-440F-BFB4-B75133F21E88}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{09C2883A-FE89-41EB-9B4F-685F7054BFF8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{09C2883A-FE89-41EB-9B4F-685F7054BFF8}"/>
   </bookViews>
   <sheets>
     <sheet name="ft4 i trab" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
-  <si>
-    <t>fT4 (pg/mL)</t>
-  </si>
   <si>
     <t>TRAb(U/mL)</t>
   </si>
@@ -71,6 +68,9 @@
   </si>
   <si>
     <t>FT4 (pg/ml)</t>
+  </si>
+  <si>
+    <t>FT4 (pg/mL)</t>
   </si>
 </sst>
 </file>
@@ -181,7 +181,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Ilości fT4 i TRAb analizowanych pacjentów</a:t>
+              <a:t>Ilości FT4 i TRAb analizowanych pacjentów</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -232,7 +232,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>fT4 (pg/mL)</c:v>
+                  <c:v>FT4 (pg/mL)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2668,29 +2668,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E740B4AC-0CE7-4C2F-ACA0-BEBF2EC352A3}">
   <dimension ref="A4:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>25.63</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <v>7.5</v>
@@ -2732,7 +2732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66936F0A-2EF8-4566-8024-ADE8A81ED3E6}">
   <dimension ref="A5:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+    <sheetView topLeftCell="E4" workbookViewId="0">
       <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
@@ -2751,27 +2751,27 @@
   <sheetData>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
         <v>4</v>
-      </c>
-      <c r="L5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>60</v>
@@ -2790,7 +2790,7 @@
         <v>360</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6">
         <f>F7/1000</f>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -2830,7 +2830,7 @@
         <v>4800</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I7" s="5">
         <v>25.63</v>
@@ -2847,7 +2847,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <f>B6*B7</f>
@@ -2868,15 +2868,15 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>90</v>
@@ -2897,7 +2897,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>40</v>
@@ -2918,7 +2918,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <f>B13*B14</f>
@@ -2939,15 +2939,15 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19">
         <v>60</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>30</v>
@@ -2989,7 +2989,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <f>B19*B20</f>
@@ -3010,15 +3010,15 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25">
         <v>60</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26">
         <v>30</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <f>B25*B26</f>

</xml_diff>